<commit_message>
feat: added legends and samples each of import templates for user reference
</commit_message>
<xml_diff>
--- a/AccuPay.Web/ImportTemplates/accupay-allowance-template.xlsx
+++ b/AccuPay.Web/ImportTemplates/accupay-allowance-template.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8355"/>
+    <workbookView windowWidth="20490" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="2" r:id="rId1"/>
-    <sheet name="Options" sheetId="3" r:id="rId2"/>
+    <sheet name="Options" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -46,12 +46,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,15 +68,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -90,17 +84,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -110,66 +104,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -181,6 +115,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -189,9 +137,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,6 +152,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -218,8 +173,46 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,13 +221,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFBBE33D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,163 +329,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,21 +418,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -461,37 +445,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -519,158 +483,197 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,6 +754,11 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="00BBE33D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1047,49 +1055,50 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E$1:E$1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="18.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="40.1428571428571" customWidth="1"/>
-    <col min="6" max="6" width="17.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="11.7142857142857" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.2857142857143" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.4285714285714" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.1428571428571" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.8571428571429" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" selectLockedCells="1" objects="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A$1:A$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E$1:E$1048576">
+      <formula1>"One time,Daily,Semi-monthly,Monthly"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
       <formula1>Options!$A$2:$A$1001</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>Options!$B$2:$B100</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E$1:E$1048576">
-      <formula1>"One time,Daily,Semi-monthly,Monthly"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1117,7 +1126,7 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>